<commit_message>
New changes  report scripts and .sql files
</commit_message>
<xml_diff>
--- a/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
+++ b/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
@@ -7,7 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="01_view_dataset_totals" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="02_view_monthly_transactions" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="24_bi_total_count_by_category_d" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="03_view_product_category_perfor" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="18_bi_top_5_max_orders_by_total" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="19_bi_top_5_min_orders_by_total" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,6 +430,665 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>total_transactions</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_customers</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_sales</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_items_sold</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>avg_age</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>avg_order_amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>456000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2514</v>
+      </c>
+      <c r="E2" t="n">
+        <v>41.392</v>
+      </c>
+      <c r="F2" t="n">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_transactions</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_sales</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_qty</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>76</v>
+      </c>
+      <c r="C2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="D2" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>85</v>
+      </c>
+      <c r="C3" t="n">
+        <v>44060</v>
+      </c>
+      <c r="D3" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>73</v>
+      </c>
+      <c r="C4" t="n">
+        <v>28990</v>
+      </c>
+      <c r="D4" t="n">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>86</v>
+      </c>
+      <c r="C5" t="n">
+        <v>33870</v>
+      </c>
+      <c r="D5" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>105</v>
+      </c>
+      <c r="C6" t="n">
+        <v>53150</v>
+      </c>
+      <c r="D6" t="n">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>77</v>
+      </c>
+      <c r="C7" t="n">
+        <v>36715</v>
+      </c>
+      <c r="D7" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>72</v>
+      </c>
+      <c r="C8" t="n">
+        <v>35465</v>
+      </c>
+      <c r="D8" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>94</v>
+      </c>
+      <c r="C9" t="n">
+        <v>36960</v>
+      </c>
+      <c r="D9" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>65</v>
+      </c>
+      <c r="C10" t="n">
+        <v>23620</v>
+      </c>
+      <c r="D10" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>96</v>
+      </c>
+      <c r="C11" t="n">
+        <v>46580</v>
+      </c>
+      <c r="D11" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>78</v>
+      </c>
+      <c r="C12" t="n">
+        <v>34920</v>
+      </c>
+      <c r="D12" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>91</v>
+      </c>
+      <c r="C13" t="n">
+        <v>44690</v>
+      </c>
+      <c r="D13" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>product_category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cnt</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>rows_with_category</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>distinct_categories</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>351</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>342</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>307</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>product_category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_sales</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_qty</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>transactions_male</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>t_quantity_male</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>t_amount_male</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>pct_t_male</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>transactions_female</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>t_quantity_female</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>t_amount_female</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>pct_t_female</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>156905</v>
+      </c>
+      <c r="C2" t="n">
+        <v>849</v>
+      </c>
+      <c r="D2" t="n">
+        <v>172</v>
+      </c>
+      <c r="E2" t="n">
+        <v>410</v>
+      </c>
+      <c r="F2" t="n">
+        <v>80170</v>
+      </c>
+      <c r="G2" t="n">
+        <v>51.09461138905707</v>
+      </c>
+      <c r="H2" t="n">
+        <v>170</v>
+      </c>
+      <c r="I2" t="n">
+        <v>439</v>
+      </c>
+      <c r="J2" t="n">
+        <v>76735</v>
+      </c>
+      <c r="K2" t="n">
+        <v>48.90538861094293</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>155580</v>
+      </c>
+      <c r="C3" t="n">
+        <v>894</v>
+      </c>
+      <c r="D3" t="n">
+        <v>177</v>
+      </c>
+      <c r="E3" t="n">
+        <v>453</v>
+      </c>
+      <c r="F3" t="n">
+        <v>74305</v>
+      </c>
+      <c r="G3" t="n">
+        <v>47.75999485795089</v>
+      </c>
+      <c r="H3" t="n">
+        <v>174</v>
+      </c>
+      <c r="I3" t="n">
+        <v>441</v>
+      </c>
+      <c r="J3" t="n">
+        <v>81275</v>
+      </c>
+      <c r="K3" t="n">
+        <v>52.24000514204911</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>143515</v>
+      </c>
+      <c r="C4" t="n">
+        <v>771</v>
+      </c>
+      <c r="D4" t="n">
+        <v>141</v>
+      </c>
+      <c r="E4" t="n">
+        <v>353</v>
+      </c>
+      <c r="F4" t="n">
+        <v>68685</v>
+      </c>
+      <c r="G4" t="n">
+        <v>47.85910880395777</v>
+      </c>
+      <c r="H4" t="n">
+        <v>166</v>
+      </c>
+      <c r="I4" t="n">
+        <v>418</v>
+      </c>
+      <c r="J4" t="n">
+        <v>74830</v>
+      </c>
+      <c r="K4" t="n">
+        <v>52.14089119604223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>total_amount</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B4" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B5" t="n">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
New master_report_pipeline.py scripts and changes to some scripts and .sql files
</commit_message>
<xml_diff>
--- a/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
+++ b/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
@@ -13,6 +13,7 @@
     <sheet name="03_view_product_category_perfor" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="18_bi_top_5_max_orders_by_total" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="19_bi_top_5_min_orders_by_total" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="17_bi_percentiles_outliers_tota" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,7 +462,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>avg_age</t>
+          <t>avg_customer_age</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -527,7 +528,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total_qty</t>
+          <t>total_qty_sold</t>
         </is>
       </c>
     </row>
@@ -766,12 +767,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>cnt</t>
+          <t>order_cnt_by_cat</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>rows_with_category</t>
+          <t>orders_by_category_totals</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -860,7 +861,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>total_qty</t>
+          <t>total_qty_sold</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1037,12 +1038,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>total_amount</t>
+          <t>top_orders_max_amount</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>total_count</t>
+          <t>total_orders_same_amount</t>
         </is>
       </c>
     </row>
@@ -1100,12 +1101,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>total_amount</t>
+          <t>top_orders_min_amount</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>total_count</t>
+          <t>total_orders_same_amount</t>
         </is>
       </c>
     </row>
@@ -1131,6 +1132,77 @@
       </c>
       <c r="B4" t="n">
         <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>non_null_count</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>p25</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>p75</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>below_p25</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>between_p25_p75</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>above_p75</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>60</v>
+      </c>
+      <c r="C2" t="n">
+        <v>900</v>
+      </c>
+      <c r="D2" t="n">
+        <v>217</v>
+      </c>
+      <c r="E2" t="n">
+        <v>581</v>
+      </c>
+      <c r="F2" t="n">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New .sql files and views, changes of kaggle_ecom_report.py no charts
</commit_message>
<xml_diff>
--- a/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
+++ b/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
@@ -14,6 +14,9 @@
     <sheet name="18_bi_top_5_max_orders_by_total" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="19_bi_top_5_min_orders_by_total" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="17_bi_percentiles_outliers_tota" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="04_view_monthly_mom" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="05_view_monthly_ytd_performance" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="06_view_sales_and_customers_mom" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -496,13 +499,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,22 +516,47 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>month_start</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>month</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>total_transactions</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>total_sales</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total_qty_sold</t>
+          <t>total_revenue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>total_units</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>unique_customers</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>mom_revenue_growth_pct</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ytd_revenue</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ytd_units</t>
         </is>
       </c>
     </row>
@@ -539,12 +567,25 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="E2" t="n">
+        <v>195</v>
+      </c>
+      <c r="F2" t="n">
         <v>76</v>
       </c>
-      <c r="C2" t="n">
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
         <v>35450</v>
       </c>
-      <c r="D2" t="n">
+      <c r="I2" t="n">
         <v>195</v>
       </c>
     </row>
@@ -555,13 +596,28 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>44060</v>
+      </c>
+      <c r="E3" t="n">
+        <v>214</v>
+      </c>
+      <c r="F3" t="n">
         <v>85</v>
       </c>
-      <c r="C3" t="n">
-        <v>44060</v>
-      </c>
-      <c r="D3" t="n">
-        <v>214</v>
+      <c r="G3" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="H3" t="n">
+        <v>79510</v>
+      </c>
+      <c r="I3" t="n">
+        <v>409</v>
       </c>
     </row>
     <row r="4">
@@ -571,13 +627,28 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>28990</v>
+      </c>
+      <c r="E4" t="n">
+        <v>194</v>
+      </c>
+      <c r="F4" t="n">
         <v>73</v>
       </c>
-      <c r="C4" t="n">
-        <v>28990</v>
-      </c>
-      <c r="D4" t="n">
-        <v>194</v>
+      <c r="G4" t="n">
+        <v>-34.2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>108500</v>
+      </c>
+      <c r="I4" t="n">
+        <v>603</v>
       </c>
     </row>
     <row r="5">
@@ -587,13 +658,28 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>33870</v>
+      </c>
+      <c r="E5" t="n">
+        <v>214</v>
+      </c>
+      <c r="F5" t="n">
         <v>86</v>
       </c>
-      <c r="C5" t="n">
-        <v>33870</v>
-      </c>
-      <c r="D5" t="n">
-        <v>214</v>
+      <c r="G5" t="n">
+        <v>16.83</v>
+      </c>
+      <c r="H5" t="n">
+        <v>142370</v>
+      </c>
+      <c r="I5" t="n">
+        <v>817</v>
       </c>
     </row>
     <row r="6">
@@ -603,13 +689,28 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>53150</v>
+      </c>
+      <c r="E6" t="n">
+        <v>259</v>
+      </c>
+      <c r="F6" t="n">
         <v>105</v>
       </c>
-      <c r="C6" t="n">
-        <v>53150</v>
-      </c>
-      <c r="D6" t="n">
-        <v>259</v>
+      <c r="G6" t="n">
+        <v>56.92</v>
+      </c>
+      <c r="H6" t="n">
+        <v>195520</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1076</v>
       </c>
     </row>
     <row r="7">
@@ -619,13 +720,28 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36715</v>
+      </c>
+      <c r="E7" t="n">
+        <v>197</v>
+      </c>
+      <c r="F7" t="n">
         <v>77</v>
       </c>
-      <c r="C7" t="n">
-        <v>36715</v>
-      </c>
-      <c r="D7" t="n">
-        <v>197</v>
+      <c r="G7" t="n">
+        <v>-30.92</v>
+      </c>
+      <c r="H7" t="n">
+        <v>232235</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1273</v>
       </c>
     </row>
     <row r="8">
@@ -635,13 +751,28 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>35465</v>
+      </c>
+      <c r="E8" t="n">
+        <v>176</v>
+      </c>
+      <c r="F8" t="n">
         <v>72</v>
       </c>
-      <c r="C8" t="n">
-        <v>35465</v>
-      </c>
-      <c r="D8" t="n">
-        <v>176</v>
+      <c r="G8" t="n">
+        <v>-3.4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>267700</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1449</v>
       </c>
     </row>
     <row r="9">
@@ -651,13 +782,28 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>36960</v>
+      </c>
+      <c r="E9" t="n">
+        <v>227</v>
+      </c>
+      <c r="F9" t="n">
         <v>94</v>
       </c>
-      <c r="C9" t="n">
-        <v>36960</v>
-      </c>
-      <c r="D9" t="n">
-        <v>227</v>
+      <c r="G9" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="H9" t="n">
+        <v>304660</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1676</v>
       </c>
     </row>
     <row r="10">
@@ -667,13 +813,28 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
+        <v>23620</v>
+      </c>
+      <c r="E10" t="n">
+        <v>170</v>
+      </c>
+      <c r="F10" t="n">
         <v>65</v>
       </c>
-      <c r="C10" t="n">
-        <v>23620</v>
-      </c>
-      <c r="D10" t="n">
-        <v>170</v>
+      <c r="G10" t="n">
+        <v>-36.09</v>
+      </c>
+      <c r="H10" t="n">
+        <v>328280</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1846</v>
       </c>
     </row>
     <row r="11">
@@ -683,13 +844,28 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>46580</v>
+      </c>
+      <c r="E11" t="n">
+        <v>252</v>
+      </c>
+      <c r="F11" t="n">
         <v>96</v>
       </c>
-      <c r="C11" t="n">
-        <v>46580</v>
-      </c>
-      <c r="D11" t="n">
-        <v>252</v>
+      <c r="G11" t="n">
+        <v>97.20999999999999</v>
+      </c>
+      <c r="H11" t="n">
+        <v>374860</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2098</v>
       </c>
     </row>
     <row r="12">
@@ -699,13 +875,28 @@
         </is>
       </c>
       <c r="B12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n">
+        <v>34920</v>
+      </c>
+      <c r="E12" t="n">
+        <v>205</v>
+      </c>
+      <c r="F12" t="n">
         <v>78</v>
       </c>
-      <c r="C12" t="n">
-        <v>34920</v>
-      </c>
-      <c r="D12" t="n">
-        <v>205</v>
+      <c r="G12" t="n">
+        <v>-25.03</v>
+      </c>
+      <c r="H12" t="n">
+        <v>409780</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2303</v>
       </c>
     </row>
     <row r="13">
@@ -715,13 +906,28 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>44690</v>
+      </c>
+      <c r="E13" t="n">
+        <v>207</v>
+      </c>
+      <c r="F13" t="n">
         <v>91</v>
       </c>
-      <c r="C13" t="n">
-        <v>44690</v>
-      </c>
-      <c r="D13" t="n">
-        <v>207</v>
+      <c r="G13" t="n">
+        <v>27.98</v>
+      </c>
+      <c r="H13" t="n">
+        <v>454470</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2510</v>
       </c>
     </row>
     <row r="14">
@@ -731,13 +937,365 @@
         </is>
       </c>
       <c r="B14" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" t="n">
         <v>2</v>
       </c>
+      <c r="G14" t="n">
+        <v>-96.58</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>month_start</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_revenue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>total_units</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>unique_customers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="E2" t="n">
+        <v>195</v>
+      </c>
+      <c r="F2" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>44060</v>
+      </c>
+      <c r="E3" t="n">
+        <v>214</v>
+      </c>
+      <c r="F3" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>28990</v>
+      </c>
+      <c r="E4" t="n">
+        <v>194</v>
+      </c>
+      <c r="F4" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>33870</v>
+      </c>
+      <c r="E5" t="n">
+        <v>214</v>
+      </c>
+      <c r="F5" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>53150</v>
+      </c>
+      <c r="E6" t="n">
+        <v>259</v>
+      </c>
+      <c r="F6" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36715</v>
+      </c>
+      <c r="E7" t="n">
+        <v>197</v>
+      </c>
+      <c r="F7" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>35465</v>
+      </c>
+      <c r="E8" t="n">
+        <v>176</v>
+      </c>
+      <c r="F8" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>36960</v>
+      </c>
+      <c r="E9" t="n">
+        <v>227</v>
+      </c>
+      <c r="F9" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
+        <v>23620</v>
+      </c>
+      <c r="E10" t="n">
+        <v>170</v>
+      </c>
+      <c r="F10" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>46580</v>
+      </c>
+      <c r="E11" t="n">
+        <v>252</v>
+      </c>
+      <c r="F11" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n">
+        <v>34920</v>
+      </c>
+      <c r="E12" t="n">
+        <v>205</v>
+      </c>
+      <c r="F12" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>44690</v>
+      </c>
+      <c r="E13" t="n">
+        <v>207</v>
+      </c>
+      <c r="F13" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2024</v>
+      </c>
       <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
         <v>1530</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1208,4 +1766,806 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>month_start</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_revenue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>total_units</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>unique_customers</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>prev_month_revenue</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>mom_revenue_growth_pct</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="E2" t="n">
+        <v>195</v>
+      </c>
+      <c r="F2" t="n">
+        <v>76</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>44060</v>
+      </c>
+      <c r="E3" t="n">
+        <v>214</v>
+      </c>
+      <c r="F3" t="n">
+        <v>85</v>
+      </c>
+      <c r="G3" t="n">
+        <v>35450</v>
+      </c>
+      <c r="H3" t="n">
+        <v>24.29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>28990</v>
+      </c>
+      <c r="E4" t="n">
+        <v>194</v>
+      </c>
+      <c r="F4" t="n">
+        <v>73</v>
+      </c>
+      <c r="G4" t="n">
+        <v>44060</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-34.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>33870</v>
+      </c>
+      <c r="E5" t="n">
+        <v>214</v>
+      </c>
+      <c r="F5" t="n">
+        <v>86</v>
+      </c>
+      <c r="G5" t="n">
+        <v>28990</v>
+      </c>
+      <c r="H5" t="n">
+        <v>16.83</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>53150</v>
+      </c>
+      <c r="E6" t="n">
+        <v>259</v>
+      </c>
+      <c r="F6" t="n">
+        <v>105</v>
+      </c>
+      <c r="G6" t="n">
+        <v>33870</v>
+      </c>
+      <c r="H6" t="n">
+        <v>56.92</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36715</v>
+      </c>
+      <c r="E7" t="n">
+        <v>197</v>
+      </c>
+      <c r="F7" t="n">
+        <v>77</v>
+      </c>
+      <c r="G7" t="n">
+        <v>53150</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-30.92</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>35465</v>
+      </c>
+      <c r="E8" t="n">
+        <v>176</v>
+      </c>
+      <c r="F8" t="n">
+        <v>72</v>
+      </c>
+      <c r="G8" t="n">
+        <v>36715</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-3.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>36960</v>
+      </c>
+      <c r="E9" t="n">
+        <v>227</v>
+      </c>
+      <c r="F9" t="n">
+        <v>94</v>
+      </c>
+      <c r="G9" t="n">
+        <v>35465</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
+        <v>23620</v>
+      </c>
+      <c r="E10" t="n">
+        <v>170</v>
+      </c>
+      <c r="F10" t="n">
+        <v>65</v>
+      </c>
+      <c r="G10" t="n">
+        <v>36960</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-36.09</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>46580</v>
+      </c>
+      <c r="E11" t="n">
+        <v>252</v>
+      </c>
+      <c r="F11" t="n">
+        <v>96</v>
+      </c>
+      <c r="G11" t="n">
+        <v>23620</v>
+      </c>
+      <c r="H11" t="n">
+        <v>97.20999999999999</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n">
+        <v>34920</v>
+      </c>
+      <c r="E12" t="n">
+        <v>205</v>
+      </c>
+      <c r="F12" t="n">
+        <v>78</v>
+      </c>
+      <c r="G12" t="n">
+        <v>46580</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-25.03</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>44690</v>
+      </c>
+      <c r="E13" t="n">
+        <v>207</v>
+      </c>
+      <c r="F13" t="n">
+        <v>91</v>
+      </c>
+      <c r="G13" t="n">
+        <v>34920</v>
+      </c>
+      <c r="H13" t="n">
+        <v>27.98</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>44690</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-96.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>month_start</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_revenue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ytd_revenue</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>total_units</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ytd_units</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="E2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="F2" t="n">
+        <v>195</v>
+      </c>
+      <c r="G2" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>44060</v>
+      </c>
+      <c r="E3" t="n">
+        <v>79510</v>
+      </c>
+      <c r="F3" t="n">
+        <v>214</v>
+      </c>
+      <c r="G3" t="n">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>28990</v>
+      </c>
+      <c r="E4" t="n">
+        <v>108500</v>
+      </c>
+      <c r="F4" t="n">
+        <v>194</v>
+      </c>
+      <c r="G4" t="n">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>33870</v>
+      </c>
+      <c r="E5" t="n">
+        <v>142370</v>
+      </c>
+      <c r="F5" t="n">
+        <v>214</v>
+      </c>
+      <c r="G5" t="n">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>53150</v>
+      </c>
+      <c r="E6" t="n">
+        <v>195520</v>
+      </c>
+      <c r="F6" t="n">
+        <v>259</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>36715</v>
+      </c>
+      <c r="E7" t="n">
+        <v>232235</v>
+      </c>
+      <c r="F7" t="n">
+        <v>197</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>35465</v>
+      </c>
+      <c r="E8" t="n">
+        <v>267700</v>
+      </c>
+      <c r="F8" t="n">
+        <v>176</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>36960</v>
+      </c>
+      <c r="E9" t="n">
+        <v>304660</v>
+      </c>
+      <c r="F9" t="n">
+        <v>227</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>23620</v>
+      </c>
+      <c r="E10" t="n">
+        <v>328280</v>
+      </c>
+      <c r="F10" t="n">
+        <v>170</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>46580</v>
+      </c>
+      <c r="E11" t="n">
+        <v>374860</v>
+      </c>
+      <c r="F11" t="n">
+        <v>252</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>34920</v>
+      </c>
+      <c r="E12" t="n">
+        <v>409780</v>
+      </c>
+      <c r="F12" t="n">
+        <v>205</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>44690</v>
+      </c>
+      <c r="E13" t="n">
+        <v>454470</v>
+      </c>
+      <c r="F13" t="n">
+        <v>207</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New .sql files and views, PowerBI Dashboard
</commit_message>
<xml_diff>
--- a/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
+++ b/report_scripts_outcome/reports/report_ecom_kaggle.xlsx
@@ -17,6 +17,8 @@
     <sheet name="04_view_monthly_mom" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="05_view_monthly_ytd_performance" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="06_view_sales_and_customers_mom" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="07_view_product_category_sales_" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="08_view_sales_and_customers_mom" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -966,6 +968,1793 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>product_category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>month_start</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>transactions_count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>month_total_amount</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>month_total_quantity</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>pct_of_category_amount</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>pct_of_category_quantity</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>pct_of_month_amount</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>pct_of_month_quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D2" t="n">
+        <v>12430</v>
+      </c>
+      <c r="E2" t="n">
+        <v>59</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0866</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0765</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.3506</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.3026</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>26</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14035</v>
+      </c>
+      <c r="E3" t="n">
+        <v>68</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0978</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0882</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.3185</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.3178</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>21</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10545</v>
+      </c>
+      <c r="E4" t="n">
+        <v>51</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0735</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.06610000000000001</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.3637</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.2629</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>29</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11905</v>
+      </c>
+      <c r="E5" t="n">
+        <v>69</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0895</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.3515</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.3224</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>28</v>
+      </c>
+      <c r="D6" t="n">
+        <v>12450</v>
+      </c>
+      <c r="E6" t="n">
+        <v>65</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0868</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0843</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.2342</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" t="n">
+        <v>10995</v>
+      </c>
+      <c r="E7" t="n">
+        <v>66</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0766</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0856</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.2995</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.335</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>27</v>
+      </c>
+      <c r="D8" t="n">
+        <v>16090</v>
+      </c>
+      <c r="E8" t="n">
+        <v>70</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1121</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.09080000000000001</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.4537</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.3977</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>24</v>
+      </c>
+      <c r="D9" t="n">
+        <v>9790</v>
+      </c>
+      <c r="E9" t="n">
+        <v>62</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0682</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0804</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.2649</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.2731</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6320</v>
+      </c>
+      <c r="E10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0649</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.2676</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.2941</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>31</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15355</v>
+      </c>
+      <c r="E11" t="n">
+        <v>83</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.1077</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.3296</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.3294</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9700</v>
+      </c>
+      <c r="E12" t="n">
+        <v>63</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.06759999999999999</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.08169999999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.2778</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3073</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>25</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12400</v>
+      </c>
+      <c r="E13" t="n">
+        <v>62</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0864</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0804</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.2775</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2995</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Beauty</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0039</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9804</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>26</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13125</v>
+      </c>
+      <c r="E15" t="n">
+        <v>72</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0844</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0805</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.3702</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3692</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>33</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14560</v>
+      </c>
+      <c r="E16" t="n">
+        <v>75</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0936</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0839</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.3305</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3505</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>38</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15065</v>
+      </c>
+      <c r="E17" t="n">
+        <v>111</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0968</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1242</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5197000000000001</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5722</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>36</v>
+      </c>
+      <c r="D18" t="n">
+        <v>13940</v>
+      </c>
+      <c r="E18" t="n">
+        <v>93</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.0896</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.4116</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4346</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>37</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17455</v>
+      </c>
+      <c r="E19" t="n">
+        <v>97</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.1122</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1085</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.3284</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.3745</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>28</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10170</v>
+      </c>
+      <c r="E20" t="n">
+        <v>67</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0654</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.07489999999999999</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.277</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.3401</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>8250</v>
+      </c>
+      <c r="E21" t="n">
+        <v>45</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0503</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.2326</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.2557</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>32</v>
+      </c>
+      <c r="D22" t="n">
+        <v>12455</v>
+      </c>
+      <c r="E22" t="n">
+        <v>78</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0801</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0872</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.337</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.3436</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>20</v>
+      </c>
+      <c r="D23" t="n">
+        <v>9975</v>
+      </c>
+      <c r="E23" t="n">
+        <v>60</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0641</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.06710000000000001</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.4223</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.3529</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>30</v>
+      </c>
+      <c r="D24" t="n">
+        <v>13315</v>
+      </c>
+      <c r="E24" t="n">
+        <v>74</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0856</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0828</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.2859</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.2937</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>26</v>
+      </c>
+      <c r="D25" t="n">
+        <v>15200</v>
+      </c>
+      <c r="E25" t="n">
+        <v>69</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0977</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.0772</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.4353</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.3366</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Clothing</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>26</v>
+      </c>
+      <c r="D26" t="n">
+        <v>12070</v>
+      </c>
+      <c r="E26" t="n">
+        <v>53</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.0776</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0593</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.2701</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.256</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>9895</v>
+      </c>
+      <c r="E27" t="n">
+        <v>64</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.0631</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.07539999999999999</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.2791</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.3282</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="n">
+        <v>15465</v>
+      </c>
+      <c r="E28" t="n">
+        <v>71</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.09859999999999999</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.08359999999999999</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.351</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.3318</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>14</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3380</v>
+      </c>
+      <c r="E29" t="n">
+        <v>32</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0215</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0377</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.1166</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.1649</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>21</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8025</v>
+      </c>
+      <c r="E30" t="n">
+        <v>52</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.0511</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.0612</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.2369</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.243</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>40</v>
+      </c>
+      <c r="D31" t="n">
+        <v>23245</v>
+      </c>
+      <c r="E31" t="n">
+        <v>97</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.1481</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.1143</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.4373</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.3745</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>24</v>
+      </c>
+      <c r="D32" t="n">
+        <v>15550</v>
+      </c>
+      <c r="E32" t="n">
+        <v>64</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.09909999999999999</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.07539999999999999</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.4235</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.3249</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>26</v>
+      </c>
+      <c r="D33" t="n">
+        <v>11125</v>
+      </c>
+      <c r="E33" t="n">
+        <v>61</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.0709</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.0718</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.3137</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.3466</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>38</v>
+      </c>
+      <c r="D34" t="n">
+        <v>14715</v>
+      </c>
+      <c r="E34" t="n">
+        <v>87</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.09379999999999999</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.1025</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.3981</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.3833</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>25</v>
+      </c>
+      <c r="D35" t="n">
+        <v>7325</v>
+      </c>
+      <c r="E35" t="n">
+        <v>60</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.0467</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.0707</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.3101</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.3529</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>35</v>
+      </c>
+      <c r="D36" t="n">
+        <v>17910</v>
+      </c>
+      <c r="E36" t="n">
+        <v>95</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.1141</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.1119</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.3845</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.377</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>27</v>
+      </c>
+      <c r="D37" t="n">
+        <v>10020</v>
+      </c>
+      <c r="E37" t="n">
+        <v>73</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.0639</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.2869</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.3561</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>40</v>
+      </c>
+      <c r="D38" t="n">
+        <v>20220</v>
+      </c>
+      <c r="E38" t="n">
+        <v>92</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.1289</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.1084</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.4525</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.4444</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>30</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.0196</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>month_start</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_revenue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>total_units</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>unique_customers</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>mom_revenue_growth_pct</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ytd_revenue</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ytd_units</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="E2" t="n">
+        <v>195</v>
+      </c>
+      <c r="F2" t="n">
+        <v>76</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>35450</v>
+      </c>
+      <c r="I2" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>44060</v>
+      </c>
+      <c r="E3" t="n">
+        <v>214</v>
+      </c>
+      <c r="F3" t="n">
+        <v>85</v>
+      </c>
+      <c r="G3" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="H3" t="n">
+        <v>79510</v>
+      </c>
+      <c r="I3" t="n">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>28990</v>
+      </c>
+      <c r="E4" t="n">
+        <v>194</v>
+      </c>
+      <c r="F4" t="n">
+        <v>73</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-34.2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>108500</v>
+      </c>
+      <c r="I4" t="n">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>33870</v>
+      </c>
+      <c r="E5" t="n">
+        <v>214</v>
+      </c>
+      <c r="F5" t="n">
+        <v>86</v>
+      </c>
+      <c r="G5" t="n">
+        <v>16.83</v>
+      </c>
+      <c r="H5" t="n">
+        <v>142370</v>
+      </c>
+      <c r="I5" t="n">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>53150</v>
+      </c>
+      <c r="E6" t="n">
+        <v>259</v>
+      </c>
+      <c r="F6" t="n">
+        <v>105</v>
+      </c>
+      <c r="G6" t="n">
+        <v>56.92</v>
+      </c>
+      <c r="H6" t="n">
+        <v>195520</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36715</v>
+      </c>
+      <c r="E7" t="n">
+        <v>197</v>
+      </c>
+      <c r="F7" t="n">
+        <v>77</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-30.92</v>
+      </c>
+      <c r="H7" t="n">
+        <v>232235</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>35465</v>
+      </c>
+      <c r="E8" t="n">
+        <v>176</v>
+      </c>
+      <c r="F8" t="n">
+        <v>72</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-3.4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>267700</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>36960</v>
+      </c>
+      <c r="E9" t="n">
+        <v>227</v>
+      </c>
+      <c r="F9" t="n">
+        <v>94</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="H9" t="n">
+        <v>304660</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
+        <v>23620</v>
+      </c>
+      <c r="E10" t="n">
+        <v>170</v>
+      </c>
+      <c r="F10" t="n">
+        <v>65</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-36.09</v>
+      </c>
+      <c r="H10" t="n">
+        <v>328280</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>46580</v>
+      </c>
+      <c r="E11" t="n">
+        <v>252</v>
+      </c>
+      <c r="F11" t="n">
+        <v>96</v>
+      </c>
+      <c r="G11" t="n">
+        <v>97.20999999999999</v>
+      </c>
+      <c r="H11" t="n">
+        <v>374860</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n">
+        <v>34920</v>
+      </c>
+      <c r="E12" t="n">
+        <v>205</v>
+      </c>
+      <c r="F12" t="n">
+        <v>78</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-25.03</v>
+      </c>
+      <c r="H12" t="n">
+        <v>409780</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>44690</v>
+      </c>
+      <c r="E13" t="n">
+        <v>207</v>
+      </c>
+      <c r="F13" t="n">
+        <v>91</v>
+      </c>
+      <c r="G13" t="n">
+        <v>27.98</v>
+      </c>
+      <c r="H13" t="n">
+        <v>454470</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-96.58</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1530</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>